<commit_message>
Updated settings template to have max stepsize, not min. Fixed bug with display of SAXE and stepsize if stepsize threshold was exceeded.
</commit_message>
<xml_diff>
--- a/templates/ECCpy_settings_template.xlsx
+++ b/templates/ECCpy_settings_template.xlsx
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t>max_std_resp_lowdose_dp</t>
-  </si>
-  <si>
-    <t>min_acceptable_doseconc_stepsize_at_EC50</t>
-  </si>
-  <si>
-    <t>min_recommended_doseconc_stepsize_at_EC50</t>
   </si>
   <si>
     <t>e.g. 10, 50 or 90 for EC10, EC50, or EC90, respectively</t>
@@ -373,6 +367,12 @@
   </si>
   <si>
     <t>User notes or comments. Not used by ECCpy.</t>
+  </si>
+  <si>
+    <t>max_acceptable_doseconc_stepsize_at_EC50</t>
+  </si>
+  <si>
+    <t>max_recommended_doseconc_stepsize_at_EC50</t>
   </si>
 </sst>
 </file>
@@ -810,7 +810,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,21 +836,21 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -861,40 +861,40 @@
         <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -905,7 +905,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -916,7 +916,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -927,29 +927,29 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
@@ -960,73 +960,73 @@
         <v>0.8</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="B14" s="1">
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="B15" s="1">
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1">
         <v>-1</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1">
         <v>0.1</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1">
         <v>-0.2</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1037,7 +1037,7 @@
         <v>1000</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1048,40 +1048,40 @@
         <v>1.2</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
         <v>0.4</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
         <v>0.45</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1092,73 +1092,73 @@
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1">
         <v>0.3</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1">
         <v>0.3</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1189,99 +1189,99 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>30</v>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>49</v>
+      <c r="E4" s="2" t="s">
+        <v>47</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="H4" s="10"/>
     </row>
@@ -1311,36 +1311,36 @@
   <sheetData>
     <row r="1" spans="1:9" s="18" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" s="12">
         <v>1</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -1349,10 +1349,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="12">
         <v>2</v>
@@ -1366,10 +1366,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="12">
         <v>3</v>
@@ -1383,10 +1383,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" s="12">
         <v>4</v>
@@ -1400,10 +1400,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C6" s="12">
         <v>5</v>
@@ -1437,42 +1437,42 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1480,23 +1480,23 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Replaced "run analysis" with "run gatherer". Split "compare_raw" into a separate file.
</commit_message>
<xml_diff>
--- a/templates/ECCpy_settings_template.xlsx
+++ b/templates/ECCpy_settings_template.xlsx
@@ -20,15 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="108">
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>input file directory</t>
@@ -220,15 +214,6 @@
     <t>short name</t>
   </si>
   <si>
-    <t>generated_data_0.xlsx</t>
-  </si>
-  <si>
-    <t>generated_data_1.xlsx</t>
-  </si>
-  <si>
-    <t>generated_data_2.xlsx</t>
-  </si>
-  <si>
     <t>D:\data</t>
   </si>
   <si>
@@ -373,6 +358,15 @@
   </si>
   <si>
     <t>max_recommended_doseconc_stepsize_at_EC50</t>
+  </si>
+  <si>
+    <t>run gatherer</t>
+  </si>
+  <si>
+    <t>User-defined variable</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -810,7 +804,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,10 +816,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
@@ -833,332 +827,332 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-    </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1">
         <v>0.8</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B14" s="1">
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B15" s="1">
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1">
         <v>-1</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1">
         <v>0.1</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1">
         <v>-0.2</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1">
         <v>1000</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1">
         <v>1.2</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
         <v>0.4</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
         <v>0.45</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1">
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1">
         <v>0.3</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1">
         <v>0.3</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1172,118 +1166,105 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="7" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" style="5" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="7" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="7" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>19</v>
+      <c r="E1" s="14" t="s">
+        <v>24</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>22</v>
+      <c r="F1" s="14" t="s">
+        <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>20</v>
+      <c r="G1" s="15" t="s">
+        <v>25</v>
       </c>
-      <c r="E1" s="14" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="C3" s="10"/>
       <c r="D3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="C4" s="10"/>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
-      <c r="H4" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1311,36 +1292,36 @@
   <sheetData>
     <row r="1" spans="1:9" s="18" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C2" s="12">
         <v>1</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -1349,10 +1330,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C3" s="12">
         <v>2</v>
@@ -1366,10 +1347,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C4" s="12">
         <v>3</v>
@@ -1383,10 +1364,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C5" s="12">
         <v>4</v>
@@ -1400,10 +1381,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C6" s="12">
         <v>5</v>
@@ -1437,66 +1418,66 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>60</v>
+      <c r="B4" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>